<commit_message>
Windows Support Added, amongst other things
</commit_message>
<xml_diff>
--- a/Summers_2013/NPL/latticeAnalyser/LagTest/lagTest.xlsx
+++ b/Summers_2013/NPL/latticeAnalyser/LagTest/lagTest.xlsx
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -93,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +635,9 @@
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>